<commit_message>
Committed both the assigment and team Attendence Report
</commit_message>
<xml_diff>
--- a/Team_Attendance_Report.xlsx
+++ b/Team_Attendance_Report.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Angular\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Angular\JSLearning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{149CCC43-527F-44C5-BC05-64767E8043DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE16049E-1A06-4D78-9EF9-DD8CA1DF4D14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{8A0FD395-D703-44CE-9B51-72B1212B76C0}"/>
   </bookViews>
@@ -24,21 +24,70 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>HP</author>
+  </authors>
+  <commentList>
+    <comment ref="I2" authorId="0" shapeId="0" xr:uid="{51F23B11-FF0C-40D6-A717-D2038E2C7E7F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>HP:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+He was unable to join call as he was in office.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E3" authorId="0" shapeId="0" xr:uid="{77D32FD5-379B-475C-9486-F5D04D75698E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>HP:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Due to personal reason he was unable to join the session.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="15">
-  <si>
-    <t xml:space="preserve">Name </t>
-  </si>
-  <si>
-    <t>Attendence</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
   <si>
-    <t>Comment</t>
-  </si>
-  <si>
     <t>Rohit Malvi</t>
   </si>
   <si>
@@ -63,26 +112,36 @@
     <t>Present</t>
   </si>
   <si>
-    <t>1st Aug</t>
-  </si>
-  <si>
     <t>Absent</t>
   </si>
   <si>
-    <t>He as unable to join the call as he was in office</t>
+    <t>Prathmesh Patil</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -105,8 +164,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -420,21 +480,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBC72CD3-7F4C-49C6-97F9-5275C74DCBDC}">
-  <dimension ref="A1:D8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBC72CD3-7F4C-49C6-97F9-5275C74DCBDC}">
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.42578125" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" customWidth="1"/>
-    <col min="4" max="4" width="29.5703125" customWidth="1"/>
+    <col min="4" max="4" width="15" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -442,93 +506,87 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
         <v>3</v>
       </c>
+      <c r="I1" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>4</v>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>45139</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>10</v>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>45140</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" t="s">
-        <v>14</v>
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added assignment and teamReportSheet
</commit_message>
<xml_diff>
--- a/Team_Attendance_Report.xlsx
+++ b/Team_Attendance_Report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Angular\JSLearning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDAD46CB-063F-4487-886C-E36B3EBAD5ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{249E5B3B-D965-4F19-B6FC-84CC6DD0D456}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1950" yWindow="1950" windowWidth="15375" windowHeight="7785" xr2:uid="{8A0FD395-D703-44CE-9B51-72B1212B76C0}"/>
   </bookViews>
@@ -126,12 +126,60 @@
         </r>
       </text>
     </comment>
+    <comment ref="E5" authorId="0" shapeId="0" xr:uid="{90C023C5-B669-41B7-BEF8-9FA6608225DE}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>HP:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Due to personal reason unable to join the session.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I5" authorId="0" shapeId="0" xr:uid="{7C656465-E728-43EA-9823-F2CA5C793A1C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>HP:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+he has not join the meeting because he has left from office very late.</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -529,10 +577,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBC72CD3-7F4C-49C6-97F9-5275C74DCBDC}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -662,6 +710,60 @@
         <v>9</v>
       </c>
     </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>45142</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>45143</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>45144</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>45145</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>45146</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>45147</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>

<commit_message>
commit Today assignment and teamReport
</commit_message>
<xml_diff>
--- a/Team_Attendance_Report.xlsx
+++ b/Team_Attendance_Report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Angular\JSLearning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DB8A5F8-45A0-4A8E-BCBC-C45A74A87256}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{203A0CC8-1EF9-4474-8E42-FB78382800B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1950" yWindow="1950" windowWidth="15375" windowHeight="7785" xr2:uid="{8A0FD395-D703-44CE-9B51-72B1212B76C0}"/>
   </bookViews>
@@ -198,12 +198,60 @@
         </r>
       </text>
     </comment>
+    <comment ref="E7" authorId="0" shapeId="0" xr:uid="{A759A2DD-C75B-4C9B-AFB4-CEE598665385}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>HP:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Due to personal reason unable to join the session.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F7" authorId="0" shapeId="0" xr:uid="{09B18482-3B8A-47CC-BFFE-7DFC367BC61D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>HP:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+he has not join the meeting because he has left from office very late.</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -604,7 +652,7 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -796,6 +844,30 @@
       <c r="A7" s="1">
         <v>45147</v>
       </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I7" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1">

</xml_diff>

<commit_message>
commited morning session files
</commit_message>
<xml_diff>
--- a/Team_Attendance_Report.xlsx
+++ b/Team_Attendance_Report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Angular\JSLearning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{203A0CC8-1EF9-4474-8E42-FB78382800B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F29D06B0-D8A0-4330-8F13-6F1E959ACC5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1950" yWindow="1950" windowWidth="15375" windowHeight="7785" xr2:uid="{8A0FD395-D703-44CE-9B51-72B1212B76C0}"/>
   </bookViews>
@@ -246,12 +246,36 @@
         </r>
       </text>
     </comment>
+    <comment ref="E8" authorId="0" shapeId="0" xr:uid="{357F01BD-39C8-4B33-A269-C3DCE349B08C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>HP:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Due to office workload unable to join the call.</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -857,7 +881,7 @@
         <v>9</v>
       </c>
       <c r="F7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G7" t="s">
         <v>8</v>
@@ -872,6 +896,30 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>45148</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8" t="s">
+        <v>8</v>
+      </c>
+      <c r="I8" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
commit nodejs and team attendance report
</commit_message>
<xml_diff>
--- a/Team_Attendance_Report.xlsx
+++ b/Team_Attendance_Report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Angular\JSLearning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F29D06B0-D8A0-4330-8F13-6F1E959ACC5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9960C8D1-677B-466F-BCDC-B8F5D27E2727}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1950" yWindow="1950" windowWidth="15375" windowHeight="7785" xr2:uid="{8A0FD395-D703-44CE-9B51-72B1212B76C0}"/>
   </bookViews>
@@ -275,7 +275,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -676,7 +676,7 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -685,8 +685,7 @@
     <col min="2" max="2" width="12.7109375" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
     <col min="5" max="5" width="14.42578125" customWidth="1"/>
-    <col min="7" max="7" width="18.42578125" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" customWidth="1"/>
+    <col min="7" max="8" width="12.7109375" customWidth="1"/>
     <col min="9" max="9" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -924,12 +923,36 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>45149</v>
+        <v>45152</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H9" t="s">
+        <v>8</v>
+      </c>
+      <c r="I9" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>45150</v>
+        <v>45153</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
session code and attendance sheet
</commit_message>
<xml_diff>
--- a/Team_Attendance_Report.xlsx
+++ b/Team_Attendance_Report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Angular\JSLearning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB84D97D-753A-4B71-999E-EDD404CE2164}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0E72846-4275-49DD-B24B-7CE67D68C73E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1950" yWindow="1950" windowWidth="15375" windowHeight="7785" xr2:uid="{8A0FD395-D703-44CE-9B51-72B1212B76C0}"/>
   </bookViews>
@@ -275,7 +275,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="12">
   <si>
     <t>Date</t>
   </si>
@@ -308,6 +308,9 @@
   </si>
   <si>
     <t>Prathmesh Patil</t>
+  </si>
+  <si>
+    <t>no meeting</t>
   </si>
 </sst>
 </file>
@@ -673,10 +676,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBC72CD3-7F4C-49C6-97F9-5275C74DCBDC}">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1066,6 +1069,93 @@
         <v>9</v>
       </c>
     </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>45157</v>
+      </c>
+      <c r="B14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" t="s">
+        <v>9</v>
+      </c>
+      <c r="G14" t="s">
+        <v>9</v>
+      </c>
+      <c r="H14" t="s">
+        <v>8</v>
+      </c>
+      <c r="I14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>45158</v>
+      </c>
+      <c r="B15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15" t="s">
+        <v>11</v>
+      </c>
+      <c r="H15" t="s">
+        <v>11</v>
+      </c>
+      <c r="I15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>45159</v>
+      </c>
+      <c r="B16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" t="s">
+        <v>11</v>
+      </c>
+      <c r="G16" t="s">
+        <v>11</v>
+      </c>
+      <c r="H16" t="s">
+        <v>11</v>
+      </c>
+      <c r="I16" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>